<commit_message>
Remove outdated recommended course from user-facing response log
</commit_message>
<xml_diff>
--- a/log/response_log.xlsx
+++ b/log/response_log.xlsx
@@ -8,19 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shin.t/Desktop/Projects/mhesi/test_result_analysis_recommendation_orchestrator_api/log/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2B58E143-1C61-E241-88DC-A67A9889EB98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CBC62A3B-F73A-654F-9705-97B1681A6150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{71E47B97-443C-F449-9D3D-356D656D0A60}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="1" xr2:uid="{71E47B97-443C-F449-9D3D-356D656D0A60}"/>
   </bookViews>
   <sheets>
     <sheet name="response_log_csv" sheetId="1" r:id="rId1"/>
+    <sheet name="response_log_csv (2)" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'response_log_csv (2)'!$A$2:$AB$23</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="81">
   <si>
     <t>test_case_no</t>
   </si>
@@ -194,12 +198,84 @@
   </si>
   <si>
     <t>num_incorrect_answers</t>
+  </si>
+  <si>
+    <t>data gathering</t>
+  </si>
+  <si>
+    <t>runtime range</t>
+  </si>
+  <si>
+    <t>30-40</t>
+  </si>
+  <si>
+    <t>20-30</t>
+  </si>
+  <si>
+    <t>40-50</t>
+  </si>
+  <si>
+    <t>num_weaknesses &lt; 5</t>
+  </si>
+  <si>
+    <t>course recommendation</t>
+  </si>
+  <si>
+    <t>&lt;10 sec</t>
+  </si>
+  <si>
+    <t>num_weaknesses &gt; 5</t>
+  </si>
+  <si>
+    <t>10-15 sec</t>
+  </si>
+  <si>
+    <t>num incorrect answers ~5/6</t>
+  </si>
+  <si>
+    <t>num incorrect answers ~10</t>
+  </si>
+  <si>
+    <t>num incorrect answers ~30</t>
+  </si>
+  <si>
+    <t>3 sec</t>
+  </si>
+  <si>
+    <t>test analysis (weakness extraction)</t>
+  </si>
+  <si>
+    <t>6-10 sec</t>
+  </si>
+  <si>
+    <t>user facing response</t>
+  </si>
+  <si>
+    <t>6-15 sec</t>
+  </si>
+  <si>
+    <t>11-25 sec</t>
+  </si>
+  <si>
+    <t>25-30 sec</t>
+  </si>
+  <si>
+    <t>show</t>
+  </si>
+  <si>
+    <t>num incorrect answers &lt; 5</t>
+  </si>
+  <si>
+    <t>num incorrect answers 5-10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -343,7 +419,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -535,6 +611,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -696,7 +790,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -713,6 +807,49 @@
     <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1090,8 +1227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{965049F0-12A0-8941-B99B-D8FF17682C97}">
   <dimension ref="A1:AA35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView zoomScale="75" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -3299,4 +3436,2025 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{882D1967-66C6-9543-B52A-D374E5C3D1B9}">
+  <dimension ref="A1:AB43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" outlineLevelCol="2" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="33.5" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="11.6640625" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="24.1640625" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="17" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="8.33203125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="3.1640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="20" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="18.6640625" style="1" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="21.6640625" style="1" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="12" max="12" width="22.1640625" style="1" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="13" max="13" width="22.1640625" style="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="14" max="14" width="17" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="25" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="23.5" style="1" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="17" max="17" width="17.6640625" style="1" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="18" max="18" width="23.5" style="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="19" max="19" width="3.33203125" style="4" customWidth="1"/>
+    <col min="20" max="20" width="22.33203125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="23.5" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="21.6640625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="23" width="22.83203125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="20.33203125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="25" max="25" width="21.6640625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="20.5" style="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="25.33203125" customWidth="1"/>
+    <col min="28" max="28" width="13.5" style="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+    </row>
+    <row r="2" spans="1:28" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB2" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="9">
+        <v>23</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="9">
+        <v>5</v>
+      </c>
+      <c r="E3" s="9">
+        <v>3</v>
+      </c>
+      <c r="F3" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="11">
+        <v>29.840499999999999</v>
+      </c>
+      <c r="K3" s="7">
+        <v>1.5773999999999999</v>
+      </c>
+      <c r="L3" s="7">
+        <v>1.0221</v>
+      </c>
+      <c r="M3" s="11">
+        <f>K3+L3</f>
+        <v>2.5994999999999999</v>
+      </c>
+      <c r="N3" s="11">
+        <v>6.1425000000000001</v>
+      </c>
+      <c r="O3" s="11">
+        <v>10.3329</v>
+      </c>
+      <c r="P3" s="6">
+        <v>0.42030000000000001</v>
+      </c>
+      <c r="Q3" s="7">
+        <v>9.2669999999999995</v>
+      </c>
+      <c r="R3" s="11">
+        <v>10.764699999999999</v>
+      </c>
+      <c r="T3" s="1">
+        <v>487</v>
+      </c>
+      <c r="U3" s="1">
+        <v>161</v>
+      </c>
+      <c r="V3" s="1">
+        <v>296</v>
+      </c>
+      <c r="W3" s="1">
+        <v>232</v>
+      </c>
+      <c r="X3" s="1">
+        <v>296</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>232</v>
+      </c>
+      <c r="Z3" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="9">
+        <v>22</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="9">
+        <v>5</v>
+      </c>
+      <c r="E4" s="9">
+        <v>3</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0.17</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4" s="11">
+        <v>24.503900000000002</v>
+      </c>
+      <c r="K4" s="7">
+        <v>1.5172000000000001</v>
+      </c>
+      <c r="L4" s="7">
+        <v>1.0229999999999999</v>
+      </c>
+      <c r="M4" s="11">
+        <f>K4+L4</f>
+        <v>2.5402</v>
+      </c>
+      <c r="N4" s="11">
+        <v>6.4363999999999999</v>
+      </c>
+      <c r="O4" s="11">
+        <v>6.0552999999999999</v>
+      </c>
+      <c r="P4" s="6">
+        <v>0.39529999999999998</v>
+      </c>
+      <c r="Q4" s="7">
+        <v>5.4214000000000002</v>
+      </c>
+      <c r="R4" s="11">
+        <v>9.4710000000000001</v>
+      </c>
+      <c r="T4" s="1">
+        <v>487</v>
+      </c>
+      <c r="U4" s="1">
+        <v>148</v>
+      </c>
+      <c r="V4" s="1">
+        <v>300</v>
+      </c>
+      <c r="W4" s="1">
+        <v>220</v>
+      </c>
+      <c r="X4" s="1">
+        <v>300</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>220</v>
+      </c>
+      <c r="Z4" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="9">
+        <v>2</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="9">
+        <v>5</v>
+      </c>
+      <c r="E5" s="9">
+        <v>3</v>
+      </c>
+      <c r="F5" s="9">
+        <v>0</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J5" s="11">
+        <v>25.857900000000001</v>
+      </c>
+      <c r="K5" s="7">
+        <v>1.6840999999999999</v>
+      </c>
+      <c r="L5" s="7">
+        <v>1.0232000000000001</v>
+      </c>
+      <c r="M5" s="11">
+        <f>K5+L5</f>
+        <v>2.7073</v>
+      </c>
+      <c r="N5" s="11">
+        <v>7.6795999999999998</v>
+      </c>
+      <c r="O5" s="11">
+        <v>8.7030999999999992</v>
+      </c>
+      <c r="P5" s="6">
+        <v>0.39910000000000001</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>8.1353000000000009</v>
+      </c>
+      <c r="R5" s="11">
+        <v>6.7605000000000004</v>
+      </c>
+      <c r="T5" s="1">
+        <v>487</v>
+      </c>
+      <c r="U5" s="1">
+        <v>160</v>
+      </c>
+      <c r="V5" s="1">
+        <v>300</v>
+      </c>
+      <c r="W5" s="1">
+        <v>207</v>
+      </c>
+      <c r="X5" s="1">
+        <v>300</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>207</v>
+      </c>
+      <c r="Z5" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="9">
+        <v>14</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="9">
+        <v>5</v>
+      </c>
+      <c r="E6" s="9">
+        <v>3</v>
+      </c>
+      <c r="F6" s="9">
+        <v>0</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" s="11">
+        <v>27.408100000000001</v>
+      </c>
+      <c r="K6" s="7">
+        <v>1.3975</v>
+      </c>
+      <c r="L6" s="7">
+        <v>0.84730000000000005</v>
+      </c>
+      <c r="M6" s="11">
+        <f>K6+L6</f>
+        <v>2.2448000000000001</v>
+      </c>
+      <c r="N6" s="11">
+        <v>7.4112</v>
+      </c>
+      <c r="O6" s="11">
+        <v>10.1774</v>
+      </c>
+      <c r="P6" s="6">
+        <v>0.41830000000000001</v>
+      </c>
+      <c r="Q6" s="7">
+        <v>8.4649000000000001</v>
+      </c>
+      <c r="R6" s="11">
+        <v>7.5739999999999998</v>
+      </c>
+      <c r="T6" s="1">
+        <v>788</v>
+      </c>
+      <c r="U6" s="1">
+        <v>268</v>
+      </c>
+      <c r="V6" s="1">
+        <v>572</v>
+      </c>
+      <c r="W6" s="1">
+        <v>460</v>
+      </c>
+      <c r="X6" s="1">
+        <v>286</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>230</v>
+      </c>
+      <c r="Z6" s="9">
+        <v>2</v>
+      </c>
+      <c r="AA6" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="9">
+        <v>15</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="9">
+        <v>5</v>
+      </c>
+      <c r="E7" s="9">
+        <v>3</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J7" s="11">
+        <v>22.1127</v>
+      </c>
+      <c r="K7" s="7">
+        <v>1.7395</v>
+      </c>
+      <c r="L7" s="7">
+        <v>1.02</v>
+      </c>
+      <c r="M7" s="11">
+        <f>K7+L7</f>
+        <v>2.7595000000000001</v>
+      </c>
+      <c r="N7" s="11">
+        <v>9.6204000000000001</v>
+      </c>
+      <c r="O7" s="11">
+        <v>4.9195000000000002</v>
+      </c>
+      <c r="P7" s="6">
+        <v>0.40550000000000003</v>
+      </c>
+      <c r="Q7" s="7">
+        <v>4.3106999999999998</v>
+      </c>
+      <c r="R7" s="11">
+        <v>4.8125999999999998</v>
+      </c>
+      <c r="T7" s="1">
+        <v>794</v>
+      </c>
+      <c r="U7" s="1">
+        <v>202</v>
+      </c>
+      <c r="V7" s="1">
+        <v>294</v>
+      </c>
+      <c r="W7" s="1">
+        <v>228</v>
+      </c>
+      <c r="X7" s="1">
+        <v>294</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>228</v>
+      </c>
+      <c r="Z7" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="9">
+        <v>4</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="9">
+        <v>5</v>
+      </c>
+      <c r="E8" s="9">
+        <v>3</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" s="11">
+        <v>29.0748</v>
+      </c>
+      <c r="K8" s="7">
+        <v>1.5277000000000001</v>
+      </c>
+      <c r="L8" s="7">
+        <v>0.92069999999999996</v>
+      </c>
+      <c r="M8" s="11">
+        <f>K8+L8</f>
+        <v>2.4483999999999999</v>
+      </c>
+      <c r="N8" s="11">
+        <v>10.7882</v>
+      </c>
+      <c r="O8" s="11">
+        <v>8.2530999999999999</v>
+      </c>
+      <c r="P8" s="6">
+        <v>0.41880000000000001</v>
+      </c>
+      <c r="Q8" s="7">
+        <v>7.6355000000000004</v>
+      </c>
+      <c r="R8" s="11">
+        <v>7.5846999999999998</v>
+      </c>
+      <c r="T8" s="1">
+        <v>855</v>
+      </c>
+      <c r="U8" s="1">
+        <v>231</v>
+      </c>
+      <c r="V8" s="1">
+        <v>289</v>
+      </c>
+      <c r="W8" s="1">
+        <v>217</v>
+      </c>
+      <c r="X8" s="1">
+        <v>289</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>217</v>
+      </c>
+      <c r="Z8" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="9">
+        <v>5</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="9">
+        <v>5</v>
+      </c>
+      <c r="E9" s="9">
+        <v>3</v>
+      </c>
+      <c r="F9" s="9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9" s="11">
+        <v>26.511099999999999</v>
+      </c>
+      <c r="K9" s="7">
+        <v>1.6244000000000001</v>
+      </c>
+      <c r="L9" s="7">
+        <v>0.9103</v>
+      </c>
+      <c r="M9" s="11">
+        <f>K9+L9</f>
+        <v>2.5347</v>
+      </c>
+      <c r="N9" s="11">
+        <v>9.8414000000000001</v>
+      </c>
+      <c r="O9" s="11">
+        <v>9.6252999999999993</v>
+      </c>
+      <c r="P9" s="6">
+        <v>0.45250000000000001</v>
+      </c>
+      <c r="Q9" s="7">
+        <v>8.077</v>
+      </c>
+      <c r="R9" s="11">
+        <v>4.5091000000000001</v>
+      </c>
+      <c r="T9" s="1">
+        <v>1135</v>
+      </c>
+      <c r="U9" s="1">
+        <v>557</v>
+      </c>
+      <c r="V9" s="1">
+        <v>1149</v>
+      </c>
+      <c r="W9" s="1">
+        <v>872</v>
+      </c>
+      <c r="X9" s="1">
+        <v>287.25</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>218</v>
+      </c>
+      <c r="Z9" s="9">
+        <v>4</v>
+      </c>
+      <c r="AA9" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="12">
+        <v>21</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="12">
+        <v>5</v>
+      </c>
+      <c r="E10" s="12">
+        <v>3</v>
+      </c>
+      <c r="F10" s="12">
+        <v>0.17</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="J10" s="13">
+        <v>36.6417</v>
+      </c>
+      <c r="K10" s="7">
+        <v>1.7568999999999999</v>
+      </c>
+      <c r="L10" s="7">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="M10" s="13">
+        <f>K10+L10</f>
+        <v>2.6948999999999996</v>
+      </c>
+      <c r="N10" s="13">
+        <v>12.5382</v>
+      </c>
+      <c r="O10" s="13">
+        <v>12.494300000000001</v>
+      </c>
+      <c r="P10" s="6">
+        <v>0.44269999999999998</v>
+      </c>
+      <c r="Q10" s="7">
+        <v>11.8475</v>
+      </c>
+      <c r="R10" s="13">
+        <v>8.9131999999999998</v>
+      </c>
+      <c r="T10" s="1">
+        <v>1162</v>
+      </c>
+      <c r="U10" s="1">
+        <v>545</v>
+      </c>
+      <c r="V10" s="1">
+        <v>1028</v>
+      </c>
+      <c r="W10" s="1">
+        <v>785</v>
+      </c>
+      <c r="X10" s="1">
+        <v>257</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>196.25</v>
+      </c>
+      <c r="Z10" s="12">
+        <v>4</v>
+      </c>
+      <c r="AA10" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="12">
+        <v>1</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="12">
+        <v>5</v>
+      </c>
+      <c r="E11" s="12">
+        <v>3</v>
+      </c>
+      <c r="F11" s="12">
+        <v>0</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="J11" s="13">
+        <v>38.019799999999996</v>
+      </c>
+      <c r="K11" s="7">
+        <v>1.79</v>
+      </c>
+      <c r="L11" s="7">
+        <v>1.0267999999999999</v>
+      </c>
+      <c r="M11" s="13">
+        <f>K11+L11</f>
+        <v>2.8167999999999997</v>
+      </c>
+      <c r="N11" s="13">
+        <v>14.771699999999999</v>
+      </c>
+      <c r="O11" s="13">
+        <v>14.437900000000001</v>
+      </c>
+      <c r="P11" s="6">
+        <v>0.432</v>
+      </c>
+      <c r="Q11" s="7">
+        <v>13.812200000000001</v>
+      </c>
+      <c r="R11" s="13">
+        <v>5.9924999999999997</v>
+      </c>
+      <c r="T11" s="1">
+        <v>1162</v>
+      </c>
+      <c r="U11" s="1">
+        <v>562</v>
+      </c>
+      <c r="V11" s="1">
+        <v>1028</v>
+      </c>
+      <c r="W11" s="1">
+        <v>814</v>
+      </c>
+      <c r="X11" s="1">
+        <v>257</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>203.5</v>
+      </c>
+      <c r="Z11" s="12">
+        <v>4</v>
+      </c>
+      <c r="AA11" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="12">
+        <v>5</v>
+      </c>
+      <c r="E12" s="12">
+        <v>3</v>
+      </c>
+      <c r="F12" s="12">
+        <v>0</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="J12" s="13">
+        <v>36.7517</v>
+      </c>
+      <c r="K12" s="7">
+        <v>1.7266999999999999</v>
+      </c>
+      <c r="L12" s="7">
+        <v>0.92249999999999999</v>
+      </c>
+      <c r="M12" s="13">
+        <f>K12+L12</f>
+        <v>2.6492</v>
+      </c>
+      <c r="N12" s="13">
+        <v>15.6648</v>
+      </c>
+      <c r="O12" s="13">
+        <v>10.7546</v>
+      </c>
+      <c r="P12" s="6">
+        <v>0.4481</v>
+      </c>
+      <c r="Q12" s="7">
+        <v>10.1648</v>
+      </c>
+      <c r="R12" s="13">
+        <v>7.6822999999999997</v>
+      </c>
+      <c r="T12" s="1">
+        <v>1158</v>
+      </c>
+      <c r="U12" s="1">
+        <v>476</v>
+      </c>
+      <c r="V12" s="1">
+        <v>1042</v>
+      </c>
+      <c r="W12" s="1">
+        <v>780</v>
+      </c>
+      <c r="X12" s="1">
+        <v>260.5</v>
+      </c>
+      <c r="Y12" s="1">
+        <v>195</v>
+      </c>
+      <c r="Z12" s="12">
+        <v>4</v>
+      </c>
+      <c r="AA12" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="12">
+        <v>3</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="12">
+        <v>5</v>
+      </c>
+      <c r="E13" s="12">
+        <v>3</v>
+      </c>
+      <c r="F13" s="12">
+        <v>0</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="J13" s="13">
+        <v>35.828200000000002</v>
+      </c>
+      <c r="K13" s="7">
+        <v>1.6232</v>
+      </c>
+      <c r="L13" s="7">
+        <v>1.0330999999999999</v>
+      </c>
+      <c r="M13" s="13">
+        <f>K13+L13</f>
+        <v>2.6562999999999999</v>
+      </c>
+      <c r="N13" s="13">
+        <v>16.8873</v>
+      </c>
+      <c r="O13" s="13">
+        <v>9.5236000000000001</v>
+      </c>
+      <c r="P13" s="6">
+        <v>0.43740000000000001</v>
+      </c>
+      <c r="Q13" s="7">
+        <v>7.9451000000000001</v>
+      </c>
+      <c r="R13" s="13">
+        <v>6.7601000000000004</v>
+      </c>
+      <c r="T13" s="1">
+        <v>1737</v>
+      </c>
+      <c r="U13" s="1">
+        <v>445</v>
+      </c>
+      <c r="V13" s="1">
+        <v>838</v>
+      </c>
+      <c r="W13" s="1">
+        <v>678</v>
+      </c>
+      <c r="X13" s="1">
+        <v>279.33333333333297</v>
+      </c>
+      <c r="Y13" s="1">
+        <v>226</v>
+      </c>
+      <c r="Z13" s="12">
+        <v>3</v>
+      </c>
+      <c r="AA13" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="15">
+        <v>8</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="15">
+        <v>5</v>
+      </c>
+      <c r="E14" s="15">
+        <v>3</v>
+      </c>
+      <c r="F14" s="15">
+        <v>0</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="J14" s="16">
+        <v>43.564700000000002</v>
+      </c>
+      <c r="K14" s="7">
+        <v>1.6375999999999999</v>
+      </c>
+      <c r="L14" s="7">
+        <v>1.0741000000000001</v>
+      </c>
+      <c r="M14" s="16">
+        <f>K14+L14</f>
+        <v>2.7117</v>
+      </c>
+      <c r="N14" s="16">
+        <v>21.645</v>
+      </c>
+      <c r="O14" s="16">
+        <v>12.289199999999999</v>
+      </c>
+      <c r="P14" s="6">
+        <v>0.44419999999999998</v>
+      </c>
+      <c r="Q14" s="7">
+        <v>10.7524</v>
+      </c>
+      <c r="R14" s="16">
+        <v>6.9180000000000001</v>
+      </c>
+      <c r="T14" s="1">
+        <v>1234</v>
+      </c>
+      <c r="U14" s="1">
+        <v>578</v>
+      </c>
+      <c r="V14" s="1">
+        <v>1425</v>
+      </c>
+      <c r="W14" s="1">
+        <v>1111</v>
+      </c>
+      <c r="X14" s="1">
+        <v>285</v>
+      </c>
+      <c r="Y14" s="1">
+        <v>222.2</v>
+      </c>
+      <c r="Z14" s="15">
+        <v>5</v>
+      </c>
+      <c r="AA14" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="9">
+        <v>7</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="9">
+        <v>5</v>
+      </c>
+      <c r="E15" s="9">
+        <v>3</v>
+      </c>
+      <c r="F15" s="9">
+        <v>0</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15" s="11">
+        <v>27.6388</v>
+      </c>
+      <c r="K15" s="7">
+        <v>1.6237999999999999</v>
+      </c>
+      <c r="L15" s="7">
+        <v>1.3385</v>
+      </c>
+      <c r="M15" s="11">
+        <f>K15+L15</f>
+        <v>2.9622999999999999</v>
+      </c>
+      <c r="N15" s="11">
+        <v>11.053800000000001</v>
+      </c>
+      <c r="O15" s="11">
+        <v>7.8822999999999999</v>
+      </c>
+      <c r="P15" s="6">
+        <v>0.41660000000000003</v>
+      </c>
+      <c r="Q15" s="7">
+        <v>7.3109000000000002</v>
+      </c>
+      <c r="R15" s="11">
+        <v>5.7397999999999998</v>
+      </c>
+      <c r="T15" s="1">
+        <v>1305</v>
+      </c>
+      <c r="U15" s="1">
+        <v>442</v>
+      </c>
+      <c r="V15" s="1">
+        <v>841</v>
+      </c>
+      <c r="W15" s="1">
+        <v>617</v>
+      </c>
+      <c r="X15" s="1">
+        <v>280.33333333333297</v>
+      </c>
+      <c r="Y15" s="1">
+        <v>205.666666666666</v>
+      </c>
+      <c r="Z15" s="9">
+        <v>3</v>
+      </c>
+      <c r="AA15" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="12">
+        <v>18</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="12">
+        <v>5</v>
+      </c>
+      <c r="E16" s="12">
+        <v>3</v>
+      </c>
+      <c r="F16" s="12">
+        <v>0</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" s="13">
+        <v>33.251600000000003</v>
+      </c>
+      <c r="K16" s="7">
+        <v>1.4234</v>
+      </c>
+      <c r="L16" s="7">
+        <v>1.0377000000000001</v>
+      </c>
+      <c r="M16" s="13">
+        <f>K16+L16</f>
+        <v>2.4611000000000001</v>
+      </c>
+      <c r="N16" s="13">
+        <v>13.706200000000001</v>
+      </c>
+      <c r="O16" s="13">
+        <v>9.2213999999999992</v>
+      </c>
+      <c r="P16" s="6">
+        <v>0.4093</v>
+      </c>
+      <c r="Q16" s="7">
+        <v>8.6508000000000003</v>
+      </c>
+      <c r="R16" s="13">
+        <v>7.8621999999999996</v>
+      </c>
+      <c r="T16" s="1">
+        <v>1328</v>
+      </c>
+      <c r="U16" s="1">
+        <v>586</v>
+      </c>
+      <c r="V16" s="1">
+        <v>1152</v>
+      </c>
+      <c r="W16" s="1">
+        <v>902</v>
+      </c>
+      <c r="X16" s="1">
+        <v>288</v>
+      </c>
+      <c r="Y16" s="1">
+        <v>225.5</v>
+      </c>
+      <c r="Z16" s="12">
+        <v>4</v>
+      </c>
+      <c r="AA16" s="14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="9">
+        <v>10</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="9">
+        <v>5</v>
+      </c>
+      <c r="E17" s="9">
+        <v>3</v>
+      </c>
+      <c r="F17" s="9">
+        <v>0</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J17" s="11">
+        <v>29.283000000000001</v>
+      </c>
+      <c r="K17" s="7">
+        <v>1.7356</v>
+      </c>
+      <c r="L17" s="7">
+        <v>0.83220000000000005</v>
+      </c>
+      <c r="M17" s="11">
+        <f>K17+L17</f>
+        <v>2.5678000000000001</v>
+      </c>
+      <c r="N17" s="11">
+        <v>11.662000000000001</v>
+      </c>
+      <c r="O17" s="11">
+        <v>9.4343000000000004</v>
+      </c>
+      <c r="P17" s="6">
+        <v>0.4345</v>
+      </c>
+      <c r="Q17" s="7">
+        <v>8.0478000000000005</v>
+      </c>
+      <c r="R17" s="11">
+        <v>5.6180000000000003</v>
+      </c>
+      <c r="T17" s="1">
+        <v>1667</v>
+      </c>
+      <c r="U17" s="1">
+        <v>676</v>
+      </c>
+      <c r="V17" s="1">
+        <v>1312</v>
+      </c>
+      <c r="W17" s="1">
+        <v>985</v>
+      </c>
+      <c r="X17" s="1">
+        <v>262.39999999999998</v>
+      </c>
+      <c r="Y17" s="1">
+        <v>197</v>
+      </c>
+      <c r="Z17" s="9">
+        <v>5</v>
+      </c>
+      <c r="AA17" s="10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="12">
+        <v>19</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="12">
+        <v>5</v>
+      </c>
+      <c r="E18" s="12">
+        <v>3</v>
+      </c>
+      <c r="F18" s="12">
+        <v>0</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="J18" s="13">
+        <v>32.470399999999998</v>
+      </c>
+      <c r="K18" s="7">
+        <v>1.3375999999999999</v>
+      </c>
+      <c r="L18" s="7">
+        <v>0.80779999999999996</v>
+      </c>
+      <c r="M18" s="13">
+        <f>K18+L18</f>
+        <v>2.1454</v>
+      </c>
+      <c r="N18" s="13">
+        <v>14.038600000000001</v>
+      </c>
+      <c r="O18" s="13">
+        <v>9.73</v>
+      </c>
+      <c r="P18" s="6">
+        <v>0.45040000000000002</v>
+      </c>
+      <c r="Q18" s="7">
+        <v>8.5277999999999992</v>
+      </c>
+      <c r="R18" s="13">
+        <v>6.5545999999999998</v>
+      </c>
+      <c r="T18" s="1">
+        <v>1746</v>
+      </c>
+      <c r="U18" s="1">
+        <v>562</v>
+      </c>
+      <c r="V18" s="1">
+        <v>1113</v>
+      </c>
+      <c r="W18" s="1">
+        <v>856</v>
+      </c>
+      <c r="X18" s="1">
+        <v>278.25</v>
+      </c>
+      <c r="Y18" s="1">
+        <v>214</v>
+      </c>
+      <c r="Z18" s="12">
+        <v>4</v>
+      </c>
+      <c r="AA18" s="14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="12">
+        <v>6</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="12">
+        <v>5</v>
+      </c>
+      <c r="E19" s="12">
+        <v>3</v>
+      </c>
+      <c r="F19" s="12">
+        <v>0</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="J19" s="13">
+        <v>35.219200000000001</v>
+      </c>
+      <c r="K19" s="7">
+        <v>1.5205</v>
+      </c>
+      <c r="L19" s="7">
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="M19" s="13">
+        <f>K19+L19</f>
+        <v>2.3864999999999998</v>
+      </c>
+      <c r="N19" s="13">
+        <v>14.188800000000001</v>
+      </c>
+      <c r="O19" s="13">
+        <v>11.678599999999999</v>
+      </c>
+      <c r="P19" s="6">
+        <v>0.3972</v>
+      </c>
+      <c r="Q19" s="7">
+        <v>10.6243</v>
+      </c>
+      <c r="R19" s="13">
+        <v>6.9645999999999999</v>
+      </c>
+      <c r="T19" s="1">
+        <v>1649</v>
+      </c>
+      <c r="U19" s="1">
+        <v>491</v>
+      </c>
+      <c r="V19" s="1">
+        <v>849</v>
+      </c>
+      <c r="W19" s="1">
+        <v>663</v>
+      </c>
+      <c r="X19" s="1">
+        <v>283</v>
+      </c>
+      <c r="Y19" s="1">
+        <v>221</v>
+      </c>
+      <c r="Z19" s="12">
+        <v>3</v>
+      </c>
+      <c r="AA19" s="14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" s="19" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="19">
+        <v>9</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="19">
+        <v>5</v>
+      </c>
+      <c r="E20" s="19">
+        <v>3</v>
+      </c>
+      <c r="F20" s="19">
+        <v>0</v>
+      </c>
+      <c r="G20" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" s="4"/>
+      <c r="I20" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="J20" s="20">
+        <v>42.935400000000001</v>
+      </c>
+      <c r="K20" s="20">
+        <v>1.7733000000000001</v>
+      </c>
+      <c r="L20" s="20">
+        <v>1.0573999999999999</v>
+      </c>
+      <c r="M20" s="20">
+        <f>K20+L20</f>
+        <v>2.8307000000000002</v>
+      </c>
+      <c r="N20" s="20">
+        <v>21.552600000000002</v>
+      </c>
+      <c r="O20" s="20">
+        <v>9.7521000000000004</v>
+      </c>
+      <c r="P20" s="21">
+        <v>0.45590000000000003</v>
+      </c>
+      <c r="Q20" s="20">
+        <v>8.1346000000000007</v>
+      </c>
+      <c r="R20" s="20">
+        <v>8.7988999999999997</v>
+      </c>
+      <c r="S20" s="4"/>
+      <c r="T20" s="19">
+        <v>1803</v>
+      </c>
+      <c r="U20" s="19">
+        <v>920</v>
+      </c>
+      <c r="V20" s="19">
+        <v>1458</v>
+      </c>
+      <c r="W20" s="19">
+        <v>1174</v>
+      </c>
+      <c r="X20" s="19">
+        <v>291.60000000000002</v>
+      </c>
+      <c r="Y20" s="19">
+        <v>234.8</v>
+      </c>
+      <c r="Z20" s="19">
+        <v>8</v>
+      </c>
+      <c r="AA20" s="22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="15">
+        <v>17</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="15">
+        <v>5</v>
+      </c>
+      <c r="E21" s="15">
+        <v>3</v>
+      </c>
+      <c r="F21" s="15">
+        <v>0</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="I21" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="J21" s="16">
+        <v>49.535699999999999</v>
+      </c>
+      <c r="K21" s="7">
+        <v>2.0184000000000002</v>
+      </c>
+      <c r="L21" s="7">
+        <v>0.96530000000000005</v>
+      </c>
+      <c r="M21" s="16">
+        <f>K21+L21</f>
+        <v>2.9837000000000002</v>
+      </c>
+      <c r="N21" s="16">
+        <v>25.7651</v>
+      </c>
+      <c r="O21" s="16">
+        <v>9.3183000000000007</v>
+      </c>
+      <c r="P21" s="6">
+        <v>0.46350000000000002</v>
+      </c>
+      <c r="Q21" s="7">
+        <v>8.0381</v>
+      </c>
+      <c r="R21" s="16">
+        <v>11.467499999999999</v>
+      </c>
+      <c r="T21" s="1">
+        <v>5553</v>
+      </c>
+      <c r="U21" s="1">
+        <v>1599</v>
+      </c>
+      <c r="V21" s="1">
+        <v>1431</v>
+      </c>
+      <c r="W21" s="1">
+        <v>1103</v>
+      </c>
+      <c r="X21" s="1">
+        <v>286.2</v>
+      </c>
+      <c r="Y21" s="1">
+        <v>220.6</v>
+      </c>
+      <c r="Z21" s="15">
+        <v>8</v>
+      </c>
+      <c r="AA21" s="17">
+        <v>30</v>
+      </c>
+      <c r="AB21" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="15">
+        <v>25</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="15">
+        <v>5</v>
+      </c>
+      <c r="E22" s="15">
+        <v>3</v>
+      </c>
+      <c r="F22" s="15">
+        <v>0</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I22" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="J22" s="16">
+        <v>50.580199999999998</v>
+      </c>
+      <c r="K22" s="7">
+        <v>1.5225</v>
+      </c>
+      <c r="L22" s="7">
+        <v>0.94840000000000002</v>
+      </c>
+      <c r="M22" s="16">
+        <f>K22+L22</f>
+        <v>2.4708999999999999</v>
+      </c>
+      <c r="N22" s="16">
+        <v>25.273800000000001</v>
+      </c>
+      <c r="O22" s="16">
+        <v>12.363</v>
+      </c>
+      <c r="P22" s="6">
+        <v>0.4556</v>
+      </c>
+      <c r="Q22" s="7">
+        <v>11.8233</v>
+      </c>
+      <c r="R22" s="16">
+        <v>10.471399999999999</v>
+      </c>
+      <c r="T22" s="1">
+        <v>5893</v>
+      </c>
+      <c r="U22" s="1">
+        <v>1568</v>
+      </c>
+      <c r="V22" s="1">
+        <v>1423</v>
+      </c>
+      <c r="W22" s="1">
+        <v>1159</v>
+      </c>
+      <c r="X22" s="1">
+        <v>284.60000000000002</v>
+      </c>
+      <c r="Y22" s="1">
+        <v>231.8</v>
+      </c>
+      <c r="Z22" s="15">
+        <v>8</v>
+      </c>
+      <c r="AA22" s="17">
+        <v>32</v>
+      </c>
+      <c r="AB22" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="15">
+        <v>26</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="15">
+        <v>5</v>
+      </c>
+      <c r="E23" s="15">
+        <v>3</v>
+      </c>
+      <c r="F23" s="15">
+        <v>0</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="I23" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="J23" s="16">
+        <v>50.623600000000003</v>
+      </c>
+      <c r="K23" s="7">
+        <v>1.7739</v>
+      </c>
+      <c r="L23" s="7">
+        <v>1.0491999999999999</v>
+      </c>
+      <c r="M23" s="16">
+        <f>K23+L23</f>
+        <v>2.8231000000000002</v>
+      </c>
+      <c r="N23" s="16">
+        <v>30.735800000000001</v>
+      </c>
+      <c r="O23" s="16">
+        <v>10.813599999999999</v>
+      </c>
+      <c r="P23" s="6">
+        <v>0.45979999999999999</v>
+      </c>
+      <c r="Q23" s="7">
+        <v>10.1661</v>
+      </c>
+      <c r="R23" s="16">
+        <v>6.2497999999999996</v>
+      </c>
+      <c r="T23" s="1">
+        <v>5893</v>
+      </c>
+      <c r="U23" s="1">
+        <v>1284</v>
+      </c>
+      <c r="V23" s="1">
+        <v>1390</v>
+      </c>
+      <c r="W23" s="1">
+        <v>1091</v>
+      </c>
+      <c r="X23" s="1">
+        <v>278</v>
+      </c>
+      <c r="Y23" s="1">
+        <v>218.2</v>
+      </c>
+      <c r="Z23" s="15">
+        <v>5</v>
+      </c>
+      <c r="AA23" s="17">
+        <v>32</v>
+      </c>
+      <c r="AB23" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J25" s="1">
+        <f>AVERAGE(J3:J23)</f>
+        <v>34.65014285714286</v>
+      </c>
+      <c r="K25" s="1">
+        <f t="shared" ref="K25:R25" si="0">AVERAGE(K3:K23)</f>
+        <v>1.6348190476190474</v>
+      </c>
+      <c r="L25" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98398095238095229</v>
+      </c>
+      <c r="N25" s="1">
+        <f t="shared" si="0"/>
+        <v>14.638257142857142</v>
+      </c>
+      <c r="O25" s="1">
+        <f t="shared" si="0"/>
+        <v>9.8933238095238085</v>
+      </c>
+      <c r="P25" s="1">
+        <f t="shared" si="0"/>
+        <v>0.43128571428571433</v>
+      </c>
+      <c r="Q25" s="1">
+        <f t="shared" si="0"/>
+        <v>8.9122619047619054</v>
+      </c>
+      <c r="R25" s="1">
+        <f t="shared" si="0"/>
+        <v>7.4985476190476179</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J26" s="1">
+        <f>MIN(J3:J23)</f>
+        <v>22.1127</v>
+      </c>
+      <c r="K26" s="1">
+        <f t="shared" ref="K26:R26" si="1">MIN(K3:K23)</f>
+        <v>1.3375999999999999</v>
+      </c>
+      <c r="L26" s="1">
+        <f t="shared" si="1"/>
+        <v>0.80779999999999996</v>
+      </c>
+      <c r="N26" s="1">
+        <f t="shared" si="1"/>
+        <v>6.1425000000000001</v>
+      </c>
+      <c r="O26" s="1">
+        <f t="shared" si="1"/>
+        <v>4.9195000000000002</v>
+      </c>
+      <c r="P26" s="1">
+        <f t="shared" si="1"/>
+        <v>0.39529999999999998</v>
+      </c>
+      <c r="Q26" s="1">
+        <f t="shared" si="1"/>
+        <v>4.3106999999999998</v>
+      </c>
+      <c r="R26" s="1">
+        <f t="shared" si="1"/>
+        <v>4.5091000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J27" s="1">
+        <f>MAX(J3:J23)</f>
+        <v>50.623600000000003</v>
+      </c>
+      <c r="K27" s="1">
+        <f t="shared" ref="K27:R27" si="2">MAX(K3:K23)</f>
+        <v>2.0184000000000002</v>
+      </c>
+      <c r="L27" s="1">
+        <f t="shared" si="2"/>
+        <v>1.3385</v>
+      </c>
+      <c r="N27" s="1">
+        <f t="shared" si="2"/>
+        <v>30.735800000000001</v>
+      </c>
+      <c r="O27" s="1">
+        <f t="shared" si="2"/>
+        <v>14.437900000000001</v>
+      </c>
+      <c r="P27" s="1">
+        <f t="shared" si="2"/>
+        <v>0.46350000000000002</v>
+      </c>
+      <c r="Q27" s="1">
+        <f t="shared" si="2"/>
+        <v>13.812200000000001</v>
+      </c>
+      <c r="R27" s="1">
+        <f t="shared" si="2"/>
+        <v>11.467499999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E29" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C31" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C33" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C34" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C35" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C38" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C39" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C40" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C41" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="3:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C42" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="3:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C43" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A2:AB23" xr:uid="{882D1967-66C6-9543-B52A-D374E5C3D1B9}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:AB23">
+      <sortCondition ref="AA2:AA23"/>
+    </sortState>
+  </autoFilter>
+  <mergeCells count="3">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="J1:R1"/>
+    <mergeCell ref="T1:Y1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>